<commit_message>
Commit all files of JenkinsRobotFramework
</commit_message>
<xml_diff>
--- a/ExcelFile/TestDataDriven.xlsx
+++ b/ExcelFile/TestDataDriven.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaush\OneDrive\Desktop\JenkinsProjectSeleniun\ExcelFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E2F487-7B91-4FF0-9986-2A0CFC9AFF53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F81FA34-1064-4A2F-BC58-14F6952D2759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>